<commit_message>
20241220 parece que las tensiones van bien
</commit_message>
<xml_diff>
--- a/datos_terreno_2.xlsx
+++ b/datos_terreno_2.xlsx
@@ -437,7 +437,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="1">
-        <v>6.5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
         <v>16</v>
@@ -452,7 +452,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="1">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>